<commit_message>
atualização caso de teste
</commit_message>
<xml_diff>
--- a/teste/Caso de Teste Mostrar Estatísticas.xlsx
+++ b/teste/Caso de Teste Mostrar Estatísticas.xlsx
@@ -8,18 +8,18 @@
   </bookViews>
   <sheets>
     <sheet name="Capa" sheetId="5" r:id="rId1"/>
-    <sheet name="Registrar Entrada-FP" sheetId="16" r:id="rId2"/>
+    <sheet name="Mostrar Estatísticas - FP" sheetId="16" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Registrar Entrada-FP'!$B$1:$T$7</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="1">'Registrar Entrada-FP'!$1:$7</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Mostrar Estatísticas - FP'!$B$1:$T$7</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">'Mostrar Estatísticas - FP'!$1:$7</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>CAMPO</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Testador:</t>
   </si>
   <si>
-    <t>DADOS DE SAÍDA</t>
-  </si>
-  <si>
     <t>&lt;versão 1.0&gt;</t>
   </si>
   <si>
@@ -81,34 +78,7 @@
     <t>CT003</t>
   </si>
   <si>
-    <t>Nome</t>
-  </si>
-  <si>
-    <t>Cpf</t>
-  </si>
-  <si>
     <t>Valdeneir Wendell</t>
-  </si>
-  <si>
-    <t>O sistema oferece a interface de entrada de veiculos.</t>
-  </si>
-  <si>
-    <t>Buscar placa de veiculo</t>
-  </si>
-  <si>
-    <t>Selecionar confirmação de registro de entrada do cliente</t>
-  </si>
-  <si>
-    <t>O sistema confirma o registro da entrada do veiculo e imprime um comprovante</t>
-  </si>
-  <si>
-    <t>O ator preenche o campo "Placa do Veiculo" e seleciona em "Consultar"</t>
-  </si>
-  <si>
-    <t>O sistema verifica pela placa do veiculo se o cliente está cadastrado e informa na tela</t>
-  </si>
-  <si>
-    <t>Após verificar os dados do cliente o ator seleciona em "Confirmar Registro"</t>
   </si>
   <si>
     <t>Tela Principal &gt; Mostrar Estatísticas de Utilização</t>
@@ -123,7 +93,34 @@
     <t>Não ter aberto anteriormente.</t>
   </si>
   <si>
-    <t xml:space="preserve">O ator seleciona </t>
+    <t>Selecionar a opção "Estatísticas de Utilização"</t>
+  </si>
+  <si>
+    <t>O sistema oferece uma interface solicitando informações para gerar estatísticas.</t>
+  </si>
+  <si>
+    <t>Buscar nome do estacionamento para gerar estatísticas.</t>
+  </si>
+  <si>
+    <t>Selecionar a opção de seleção dos nomes dos estacionamentos e digitar o nome do estacionamento desejado.</t>
+  </si>
+  <si>
+    <t>O sistema exibe os nomes dos estacionamentos cadastrados, com a opção de filtragem por nome.</t>
+  </si>
+  <si>
+    <t>Selecionar estacionamento para exibir gráfico.</t>
+  </si>
+  <si>
+    <t>Selecionar o estacionamento desejado e clicar em exibir gráfico.</t>
+  </si>
+  <si>
+    <t>O sistema exibe um gráfico com a quantidade de reservas de estacionamentos de acordo com o tipo de reserva registrado na base de dados de reserva de vagas.</t>
+  </si>
+  <si>
+    <t>Resultado</t>
+  </si>
+  <si>
+    <t>Passou</t>
   </si>
 </sst>
 </file>
@@ -133,7 +130,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;CT&quot;000"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -229,6 +226,28 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -900,7 +919,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="155">
+  <cellXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1061,9 +1080,6 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="10" fillId="8" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1078,9 +1094,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="43" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1140,6 +1153,129 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="32" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="36" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="46" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1149,15 +1285,6 @@
     <xf numFmtId="0" fontId="10" fillId="8" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1176,12 +1303,6 @@
     <xf numFmtId="0" fontId="10" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1191,121 +1312,25 @@
     <xf numFmtId="0" fontId="10" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="43" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="32" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="36" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="46" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1839,11 +1864,11 @@
       <c r="B13" s="3"/>
       <c r="C13" s="4"/>
       <c r="D13" s="13"/>
-      <c r="E13" s="97" t="s">
+      <c r="E13" s="95" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="97"/>
-      <c r="G13" s="97"/>
+      <c r="F13" s="95"/>
+      <c r="G13" s="95"/>
       <c r="H13" s="14"/>
       <c r="I13" s="4"/>
       <c r="J13" s="8"/>
@@ -1852,9 +1877,9 @@
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
       <c r="D14" s="13"/>
-      <c r="E14" s="97"/>
-      <c r="F14" s="97"/>
-      <c r="G14" s="97"/>
+      <c r="E14" s="95"/>
+      <c r="F14" s="95"/>
+      <c r="G14" s="95"/>
       <c r="H14" s="14"/>
       <c r="I14" s="4"/>
       <c r="J14" s="8"/>
@@ -1874,11 +1899,11 @@
       <c r="B16" s="3"/>
       <c r="C16" s="4"/>
       <c r="D16" s="13"/>
-      <c r="E16" s="98" t="s">
-        <v>17</v>
+      <c r="E16" s="96" t="s">
+        <v>16</v>
       </c>
-      <c r="F16" s="98"/>
-      <c r="G16" s="98"/>
+      <c r="F16" s="96"/>
+      <c r="G16" s="96"/>
       <c r="H16" s="14"/>
       <c r="I16" s="4"/>
       <c r="J16" s="8"/>
@@ -1887,9 +1912,9 @@
       <c r="B17" s="3"/>
       <c r="C17" s="4"/>
       <c r="D17" s="13"/>
-      <c r="E17" s="98"/>
-      <c r="F17" s="98"/>
-      <c r="G17" s="98"/>
+      <c r="E17" s="96"/>
+      <c r="F17" s="96"/>
+      <c r="G17" s="96"/>
       <c r="H17" s="14"/>
       <c r="I17" s="4"/>
       <c r="J17" s="8"/>
@@ -1900,7 +1925,7 @@
       <c r="D18" s="13"/>
       <c r="E18" s="18"/>
       <c r="F18" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G18" s="18"/>
       <c r="H18" s="14"/>
@@ -1937,7 +1962,7 @@
       <c r="D21" s="13"/>
       <c r="E21" s="18"/>
       <c r="F21" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G21" s="18"/>
       <c r="H21" s="14"/>
@@ -1950,7 +1975,7 @@
       <c r="D22" s="13"/>
       <c r="E22" s="18"/>
       <c r="F22" s="20" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G22" s="18"/>
       <c r="H22" s="14"/>
@@ -2119,7 +2144,7 @@
       <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomRight" activeCell="D18" sqref="D18:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2147,33 +2172,31 @@
       <c r="A1" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="108" t="s">
-        <v>17</v>
+      <c r="B1" s="144" t="s">
+        <v>16</v>
       </c>
-      <c r="C1" s="108"/>
-      <c r="D1" s="108"/>
-      <c r="E1" s="109" t="s">
+      <c r="C1" s="144"/>
+      <c r="D1" s="144"/>
+      <c r="E1" s="145" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="110" t="s">
+      <c r="F1" s="146" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="110"/>
-      <c r="H1" s="110"/>
-      <c r="I1" s="110"/>
-      <c r="J1" s="110"/>
-      <c r="K1" s="110"/>
+      <c r="G1" s="146"/>
+      <c r="H1" s="146"/>
+      <c r="I1" s="146"/>
+      <c r="J1" s="146"/>
+      <c r="K1" s="146"/>
       <c r="L1" s="67"/>
-      <c r="M1" s="99" t="s">
-        <v>15</v>
-      </c>
-      <c r="N1" s="100"/>
-      <c r="O1" s="100"/>
-      <c r="P1" s="100"/>
-      <c r="Q1" s="100"/>
-      <c r="R1" s="100"/>
-      <c r="S1" s="100"/>
-      <c r="T1" s="101"/>
+      <c r="M1" s="138"/>
+      <c r="N1" s="139"/>
+      <c r="O1" s="139"/>
+      <c r="P1" s="139"/>
+      <c r="Q1" s="139"/>
+      <c r="R1" s="139"/>
+      <c r="S1" s="139"/>
+      <c r="T1" s="140"/>
       <c r="U1" s="32"/>
       <c r="V1" s="32"/>
       <c r="W1" s="32"/>
@@ -2403,31 +2426,29 @@
       <c r="A2" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="111" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="111"/>
-      <c r="D2" s="111"/>
-      <c r="E2" s="109"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="112"/>
-      <c r="H2" s="112"/>
-      <c r="I2" s="112"/>
-      <c r="J2" s="112"/>
-      <c r="K2" s="113"/>
-      <c r="L2" s="125"/>
-      <c r="M2" s="102"/>
-      <c r="N2" s="116" t="s">
+      <c r="B2" s="134" t="s">
         <v>20</v>
       </c>
-      <c r="O2" s="116" t="s">
-        <v>21</v>
+      <c r="C2" s="134"/>
+      <c r="D2" s="134"/>
+      <c r="E2" s="145"/>
+      <c r="F2" s="136"/>
+      <c r="G2" s="136"/>
+      <c r="H2" s="136"/>
+      <c r="I2" s="136"/>
+      <c r="J2" s="136"/>
+      <c r="K2" s="147"/>
+      <c r="L2" s="137"/>
+      <c r="M2" s="150" t="s">
+        <v>32</v>
       </c>
-      <c r="P2" s="116"/>
-      <c r="Q2" s="116"/>
-      <c r="R2" s="116"/>
-      <c r="S2" s="116"/>
-      <c r="T2" s="105"/>
+      <c r="N2" s="130"/>
+      <c r="O2" s="130"/>
+      <c r="P2" s="130"/>
+      <c r="Q2" s="130"/>
+      <c r="R2" s="130"/>
+      <c r="S2" s="130"/>
+      <c r="T2" s="141"/>
       <c r="U2" s="32"/>
       <c r="V2" s="32"/>
       <c r="W2" s="32"/>
@@ -2658,27 +2679,27 @@
       <c r="A3" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="111" t="s">
-        <v>18</v>
+      <c r="B3" s="134" t="s">
+        <v>17</v>
       </c>
-      <c r="C3" s="111"/>
-      <c r="D3" s="111"/>
-      <c r="E3" s="109"/>
-      <c r="F3" s="112"/>
-      <c r="G3" s="112"/>
-      <c r="H3" s="112"/>
-      <c r="I3" s="112"/>
-      <c r="J3" s="112"/>
-      <c r="K3" s="114"/>
-      <c r="L3" s="125"/>
-      <c r="M3" s="103"/>
-      <c r="N3" s="117"/>
-      <c r="O3" s="117"/>
-      <c r="P3" s="117"/>
-      <c r="Q3" s="117"/>
-      <c r="R3" s="117"/>
-      <c r="S3" s="117"/>
-      <c r="T3" s="106"/>
+      <c r="C3" s="134"/>
+      <c r="D3" s="134"/>
+      <c r="E3" s="145"/>
+      <c r="F3" s="136"/>
+      <c r="G3" s="136"/>
+      <c r="H3" s="136"/>
+      <c r="I3" s="136"/>
+      <c r="J3" s="136"/>
+      <c r="K3" s="148"/>
+      <c r="L3" s="137"/>
+      <c r="M3" s="151"/>
+      <c r="N3" s="131"/>
+      <c r="O3" s="131"/>
+      <c r="P3" s="131"/>
+      <c r="Q3" s="131"/>
+      <c r="R3" s="131"/>
+      <c r="S3" s="131"/>
+      <c r="T3" s="142"/>
       <c r="U3" s="32"/>
       <c r="V3" s="32"/>
       <c r="W3" s="32"/>
@@ -2906,30 +2927,30 @@
       <c r="IK3" s="32"/>
     </row>
     <row r="4" spans="1:246" s="40" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="119" t="s">
+      <c r="A4" s="133" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="111" t="s">
-        <v>31</v>
+      <c r="B4" s="134" t="s">
+        <v>21</v>
       </c>
-      <c r="C4" s="111"/>
-      <c r="D4" s="111"/>
-      <c r="E4" s="109"/>
-      <c r="F4" s="112"/>
-      <c r="G4" s="112"/>
-      <c r="H4" s="112"/>
-      <c r="I4" s="112"/>
-      <c r="J4" s="112"/>
-      <c r="K4" s="114"/>
-      <c r="L4" s="125"/>
-      <c r="M4" s="103"/>
-      <c r="N4" s="117"/>
-      <c r="O4" s="117"/>
-      <c r="P4" s="117"/>
-      <c r="Q4" s="117"/>
-      <c r="R4" s="117"/>
-      <c r="S4" s="117"/>
-      <c r="T4" s="106"/>
+      <c r="C4" s="134"/>
+      <c r="D4" s="134"/>
+      <c r="E4" s="145"/>
+      <c r="F4" s="136"/>
+      <c r="G4" s="136"/>
+      <c r="H4" s="136"/>
+      <c r="I4" s="136"/>
+      <c r="J4" s="136"/>
+      <c r="K4" s="148"/>
+      <c r="L4" s="137"/>
+      <c r="M4" s="151"/>
+      <c r="N4" s="131"/>
+      <c r="O4" s="131"/>
+      <c r="P4" s="131"/>
+      <c r="Q4" s="131"/>
+      <c r="R4" s="131"/>
+      <c r="S4" s="131"/>
+      <c r="T4" s="142"/>
       <c r="U4" s="32"/>
       <c r="V4" s="32"/>
       <c r="W4" s="32"/>
@@ -3157,26 +3178,26 @@
       <c r="IK4" s="32"/>
     </row>
     <row r="5" spans="1:246" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="119"/>
-      <c r="B5" s="111"/>
-      <c r="C5" s="111"/>
-      <c r="D5" s="111"/>
-      <c r="E5" s="109"/>
-      <c r="F5" s="112"/>
-      <c r="G5" s="112"/>
-      <c r="H5" s="112"/>
-      <c r="I5" s="112"/>
-      <c r="J5" s="112"/>
-      <c r="K5" s="115"/>
-      <c r="L5" s="125"/>
-      <c r="M5" s="104"/>
-      <c r="N5" s="118"/>
-      <c r="O5" s="118"/>
-      <c r="P5" s="118"/>
-      <c r="Q5" s="118"/>
-      <c r="R5" s="118"/>
-      <c r="S5" s="118"/>
-      <c r="T5" s="107"/>
+      <c r="A5" s="133"/>
+      <c r="B5" s="134"/>
+      <c r="C5" s="134"/>
+      <c r="D5" s="134"/>
+      <c r="E5" s="145"/>
+      <c r="F5" s="136"/>
+      <c r="G5" s="136"/>
+      <c r="H5" s="136"/>
+      <c r="I5" s="136"/>
+      <c r="J5" s="136"/>
+      <c r="K5" s="149"/>
+      <c r="L5" s="137"/>
+      <c r="M5" s="152"/>
+      <c r="N5" s="132"/>
+      <c r="O5" s="132"/>
+      <c r="P5" s="132"/>
+      <c r="Q5" s="132"/>
+      <c r="R5" s="132"/>
+      <c r="S5" s="132"/>
+      <c r="T5" s="143"/>
       <c r="U5" s="32"/>
       <c r="V5" s="32"/>
       <c r="W5" s="32"/>
@@ -3416,14 +3437,14 @@
       <c r="J6" s="37"/>
       <c r="K6" s="37"/>
       <c r="L6" s="37"/>
-      <c r="M6" s="94"/>
-      <c r="N6" s="95"/>
-      <c r="O6" s="95"/>
-      <c r="P6" s="95"/>
-      <c r="Q6" s="95"/>
-      <c r="R6" s="95"/>
-      <c r="S6" s="95"/>
-      <c r="T6" s="96"/>
+      <c r="M6" s="92"/>
+      <c r="N6" s="93"/>
+      <c r="O6" s="93"/>
+      <c r="P6" s="93"/>
+      <c r="Q6" s="93"/>
+      <c r="R6" s="93"/>
+      <c r="S6" s="93"/>
+      <c r="T6" s="94"/>
       <c r="U6" s="32"/>
       <c r="V6" s="32"/>
       <c r="W6" s="32"/>
@@ -3911,16 +3932,16 @@
         <v>12</v>
       </c>
       <c r="B8" s="51" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C8" s="51" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D8" s="52" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="E8" s="52" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F8" s="57"/>
       <c r="G8" s="30"/>
@@ -3929,14 +3950,16 @@
       <c r="J8" s="30"/>
       <c r="K8" s="30"/>
       <c r="L8" s="63"/>
-      <c r="M8" s="76"/>
-      <c r="N8" s="77"/>
-      <c r="O8" s="78"/>
-      <c r="P8" s="78"/>
-      <c r="Q8" s="78"/>
-      <c r="R8" s="78"/>
-      <c r="S8" s="78"/>
-      <c r="T8" s="79"/>
+      <c r="M8" s="154" t="s">
+        <v>33</v>
+      </c>
+      <c r="N8" s="75"/>
+      <c r="O8" s="76"/>
+      <c r="P8" s="76"/>
+      <c r="Q8" s="76"/>
+      <c r="R8" s="76"/>
+      <c r="S8" s="76"/>
+      <c r="T8" s="77"/>
       <c r="U8" s="27"/>
       <c r="V8" s="26"/>
       <c r="W8" s="26"/>
@@ -4177,21 +4200,21 @@
       <c r="J9" s="22"/>
       <c r="K9" s="22"/>
       <c r="L9" s="22"/>
-      <c r="M9" s="73"/>
-      <c r="N9" s="74"/>
-      <c r="O9" s="74"/>
-      <c r="P9" s="74"/>
-      <c r="Q9" s="74"/>
-      <c r="R9" s="74"/>
-      <c r="S9" s="74"/>
-      <c r="T9" s="75"/>
+      <c r="M9" s="72"/>
+      <c r="N9" s="73"/>
+      <c r="O9" s="73"/>
+      <c r="P9" s="73"/>
+      <c r="Q9" s="73"/>
+      <c r="R9" s="73"/>
+      <c r="S9" s="73"/>
+      <c r="T9" s="74"/>
     </row>
     <row r="10" spans="1:246" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="59" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="51" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C10" s="52" t="s">
         <v>12</v>
@@ -4209,14 +4232,16 @@
       <c r="J10" s="28"/>
       <c r="K10" s="28"/>
       <c r="L10" s="64"/>
-      <c r="M10" s="70"/>
-      <c r="N10" s="71"/>
-      <c r="O10" s="71"/>
-      <c r="P10" s="71"/>
-      <c r="Q10" s="71"/>
-      <c r="R10" s="71"/>
-      <c r="S10" s="71"/>
-      <c r="T10" s="72"/>
+      <c r="M10" s="153" t="s">
+        <v>33</v>
+      </c>
+      <c r="N10" s="70"/>
+      <c r="O10" s="70"/>
+      <c r="P10" s="70"/>
+      <c r="Q10" s="70"/>
+      <c r="R10" s="70"/>
+      <c r="S10" s="70"/>
+      <c r="T10" s="71"/>
       <c r="U10" s="26"/>
       <c r="V10" s="26"/>
       <c r="W10" s="26"/>
@@ -4456,46 +4481,48 @@
       <c r="J11" s="22"/>
       <c r="K11" s="22"/>
       <c r="L11" s="22"/>
-      <c r="M11" s="80"/>
+      <c r="M11" s="78"/>
       <c r="N11" s="69"/>
       <c r="O11" s="69"/>
       <c r="P11" s="69"/>
       <c r="Q11" s="69"/>
       <c r="R11" s="69"/>
       <c r="S11" s="69"/>
-      <c r="T11" s="81"/>
+      <c r="T11" s="79"/>
     </row>
     <row r="12" spans="1:246" ht="52.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="120" t="s">
-        <v>19</v>
+      <c r="A12" s="127" t="s">
+        <v>18</v>
       </c>
-      <c r="B12" s="122" t="s">
-        <v>25</v>
+      <c r="B12" s="116" t="s">
+        <v>29</v>
       </c>
-      <c r="C12" s="122" t="s">
+      <c r="C12" s="116" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="122" t="s">
-        <v>29</v>
+      <c r="D12" s="116" t="s">
+        <v>30</v>
       </c>
-      <c r="E12" s="123" t="s">
-        <v>26</v>
+      <c r="E12" s="126" t="s">
+        <v>31</v>
       </c>
-      <c r="F12" s="128"/>
-      <c r="G12" s="128"/>
-      <c r="H12" s="130"/>
-      <c r="I12" s="128"/>
-      <c r="J12" s="128"/>
-      <c r="K12" s="128"/>
-      <c r="L12" s="135"/>
-      <c r="M12" s="137"/>
-      <c r="N12" s="126"/>
-      <c r="O12" s="153"/>
-      <c r="P12" s="126"/>
-      <c r="Q12" s="126"/>
-      <c r="R12" s="126"/>
-      <c r="S12" s="149"/>
-      <c r="T12" s="82"/>
+      <c r="F12" s="113"/>
+      <c r="G12" s="113"/>
+      <c r="H12" s="129"/>
+      <c r="I12" s="113"/>
+      <c r="J12" s="113"/>
+      <c r="K12" s="113"/>
+      <c r="L12" s="105"/>
+      <c r="M12" s="155" t="s">
+        <v>33</v>
+      </c>
+      <c r="N12" s="103"/>
+      <c r="O12" s="111"/>
+      <c r="P12" s="103"/>
+      <c r="Q12" s="103"/>
+      <c r="R12" s="103"/>
+      <c r="S12" s="99"/>
+      <c r="T12" s="80"/>
       <c r="U12" s="26"/>
       <c r="V12" s="26"/>
       <c r="W12" s="26"/>
@@ -4721,27 +4748,27 @@
       <c r="II12" s="26"/>
       <c r="IJ12" s="26"/>
     </row>
-    <row r="13" spans="1:246" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="121"/>
-      <c r="B13" s="122"/>
-      <c r="C13" s="122"/>
-      <c r="D13" s="122"/>
-      <c r="E13" s="124"/>
-      <c r="F13" s="129"/>
-      <c r="G13" s="129"/>
-      <c r="H13" s="129"/>
-      <c r="I13" s="129"/>
-      <c r="J13" s="129"/>
-      <c r="K13" s="129"/>
-      <c r="L13" s="136"/>
-      <c r="M13" s="138"/>
-      <c r="N13" s="127"/>
-      <c r="O13" s="154"/>
-      <c r="P13" s="127"/>
-      <c r="Q13" s="127"/>
-      <c r="R13" s="127"/>
-      <c r="S13" s="150"/>
-      <c r="T13" s="83"/>
+    <row r="13" spans="1:246" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="128"/>
+      <c r="B13" s="116"/>
+      <c r="C13" s="116"/>
+      <c r="D13" s="116"/>
+      <c r="E13" s="135"/>
+      <c r="F13" s="114"/>
+      <c r="G13" s="114"/>
+      <c r="H13" s="114"/>
+      <c r="I13" s="114"/>
+      <c r="J13" s="114"/>
+      <c r="K13" s="114"/>
+      <c r="L13" s="106"/>
+      <c r="M13" s="156"/>
+      <c r="N13" s="104"/>
+      <c r="O13" s="112"/>
+      <c r="P13" s="104"/>
+      <c r="Q13" s="104"/>
+      <c r="R13" s="104"/>
+      <c r="S13" s="100"/>
+      <c r="T13" s="81"/>
       <c r="U13" s="26"/>
       <c r="V13" s="26"/>
       <c r="W13" s="26"/>
@@ -4980,36 +5007,36 @@
       <c r="J14" s="22"/>
       <c r="K14" s="22"/>
       <c r="L14" s="22"/>
-      <c r="M14" s="84"/>
-      <c r="N14" s="77"/>
-      <c r="O14" s="77"/>
-      <c r="P14" s="77"/>
-      <c r="Q14" s="77"/>
-      <c r="R14" s="77"/>
-      <c r="S14" s="85"/>
-      <c r="T14" s="86"/>
+      <c r="M14" s="82"/>
+      <c r="N14" s="75"/>
+      <c r="O14" s="75"/>
+      <c r="P14" s="75"/>
+      <c r="Q14" s="75"/>
+      <c r="R14" s="75"/>
+      <c r="S14" s="83"/>
+      <c r="T14" s="84"/>
     </row>
     <row r="15" spans="1:246" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="120"/>
-      <c r="B15" s="122"/>
-      <c r="C15" s="122"/>
-      <c r="D15" s="122"/>
-      <c r="E15" s="131"/>
-      <c r="F15" s="128"/>
-      <c r="G15" s="128"/>
-      <c r="H15" s="128"/>
-      <c r="I15" s="128"/>
-      <c r="J15" s="128"/>
-      <c r="K15" s="128"/>
-      <c r="L15" s="135"/>
-      <c r="M15" s="137"/>
-      <c r="N15" s="126"/>
-      <c r="O15" s="153"/>
-      <c r="P15" s="126"/>
-      <c r="Q15" s="126"/>
-      <c r="R15" s="126"/>
-      <c r="S15" s="149"/>
-      <c r="T15" s="151"/>
+      <c r="A15" s="127"/>
+      <c r="B15" s="116"/>
+      <c r="C15" s="116"/>
+      <c r="D15" s="116"/>
+      <c r="E15" s="117"/>
+      <c r="F15" s="113"/>
+      <c r="G15" s="113"/>
+      <c r="H15" s="113"/>
+      <c r="I15" s="113"/>
+      <c r="J15" s="113"/>
+      <c r="K15" s="113"/>
+      <c r="L15" s="105"/>
+      <c r="M15" s="107"/>
+      <c r="N15" s="103"/>
+      <c r="O15" s="111"/>
+      <c r="P15" s="103"/>
+      <c r="Q15" s="103"/>
+      <c r="R15" s="103"/>
+      <c r="S15" s="99"/>
+      <c r="T15" s="101"/>
       <c r="U15" s="26"/>
       <c r="V15" s="26"/>
       <c r="W15" s="26"/>
@@ -5236,26 +5263,26 @@
       <c r="IJ15" s="26"/>
     </row>
     <row r="16" spans="1:246" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="121"/>
-      <c r="B16" s="122"/>
-      <c r="C16" s="122"/>
-      <c r="D16" s="122"/>
-      <c r="E16" s="132"/>
-      <c r="F16" s="129"/>
-      <c r="G16" s="129"/>
-      <c r="H16" s="129"/>
-      <c r="I16" s="129"/>
-      <c r="J16" s="129"/>
-      <c r="K16" s="129"/>
-      <c r="L16" s="136"/>
-      <c r="M16" s="138"/>
-      <c r="N16" s="127"/>
-      <c r="O16" s="154"/>
-      <c r="P16" s="127"/>
-      <c r="Q16" s="127"/>
-      <c r="R16" s="127"/>
-      <c r="S16" s="150"/>
-      <c r="T16" s="152"/>
+      <c r="A16" s="128"/>
+      <c r="B16" s="116"/>
+      <c r="C16" s="116"/>
+      <c r="D16" s="116"/>
+      <c r="E16" s="118"/>
+      <c r="F16" s="114"/>
+      <c r="G16" s="114"/>
+      <c r="H16" s="114"/>
+      <c r="I16" s="114"/>
+      <c r="J16" s="114"/>
+      <c r="K16" s="114"/>
+      <c r="L16" s="106"/>
+      <c r="M16" s="108"/>
+      <c r="N16" s="104"/>
+      <c r="O16" s="112"/>
+      <c r="P16" s="104"/>
+      <c r="Q16" s="104"/>
+      <c r="R16" s="104"/>
+      <c r="S16" s="100"/>
+      <c r="T16" s="102"/>
       <c r="U16" s="26"/>
       <c r="V16" s="26"/>
       <c r="W16" s="26"/>
@@ -5494,36 +5521,36 @@
       <c r="J17" s="47"/>
       <c r="K17" s="47"/>
       <c r="L17" s="47"/>
-      <c r="M17" s="84"/>
-      <c r="N17" s="77"/>
-      <c r="O17" s="77"/>
-      <c r="P17" s="77"/>
-      <c r="Q17" s="77"/>
-      <c r="R17" s="77"/>
-      <c r="S17" s="85"/>
-      <c r="T17" s="86"/>
+      <c r="M17" s="82"/>
+      <c r="N17" s="75"/>
+      <c r="O17" s="75"/>
+      <c r="P17" s="75"/>
+      <c r="Q17" s="75"/>
+      <c r="R17" s="75"/>
+      <c r="S17" s="83"/>
+      <c r="T17" s="84"/>
     </row>
     <row r="18" spans="1:244" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="141"/>
-      <c r="B18" s="123"/>
-      <c r="C18" s="122"/>
-      <c r="D18" s="123"/>
-      <c r="E18" s="123"/>
-      <c r="F18" s="133"/>
-      <c r="G18" s="133"/>
-      <c r="H18" s="142"/>
-      <c r="I18" s="133"/>
-      <c r="J18" s="133"/>
-      <c r="K18" s="133"/>
-      <c r="L18" s="143"/>
-      <c r="M18" s="145"/>
-      <c r="N18" s="139"/>
-      <c r="O18" s="139"/>
-      <c r="P18" s="139"/>
-      <c r="Q18" s="139"/>
-      <c r="R18" s="139"/>
-      <c r="S18" s="149"/>
-      <c r="T18" s="151"/>
+      <c r="A18" s="115"/>
+      <c r="B18" s="126"/>
+      <c r="C18" s="116"/>
+      <c r="D18" s="126"/>
+      <c r="E18" s="126"/>
+      <c r="F18" s="121"/>
+      <c r="G18" s="121"/>
+      <c r="H18" s="119"/>
+      <c r="I18" s="121"/>
+      <c r="J18" s="121"/>
+      <c r="K18" s="121"/>
+      <c r="L18" s="122"/>
+      <c r="M18" s="124"/>
+      <c r="N18" s="109"/>
+      <c r="O18" s="109"/>
+      <c r="P18" s="109"/>
+      <c r="Q18" s="109"/>
+      <c r="R18" s="109"/>
+      <c r="S18" s="99"/>
+      <c r="T18" s="101"/>
       <c r="U18" s="26"/>
       <c r="V18" s="26"/>
       <c r="W18" s="26"/>
@@ -5750,26 +5777,26 @@
       <c r="IJ18" s="26"/>
     </row>
     <row r="19" spans="1:244" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="141"/>
-      <c r="B19" s="132"/>
-      <c r="C19" s="122"/>
-      <c r="D19" s="132"/>
-      <c r="E19" s="132"/>
-      <c r="F19" s="134"/>
-      <c r="G19" s="134"/>
-      <c r="H19" s="134"/>
-      <c r="I19" s="134"/>
-      <c r="J19" s="134"/>
-      <c r="K19" s="134"/>
-      <c r="L19" s="144"/>
-      <c r="M19" s="146"/>
-      <c r="N19" s="140"/>
-      <c r="O19" s="140"/>
-      <c r="P19" s="140"/>
-      <c r="Q19" s="140"/>
-      <c r="R19" s="140"/>
-      <c r="S19" s="150"/>
-      <c r="T19" s="152"/>
+      <c r="A19" s="115"/>
+      <c r="B19" s="118"/>
+      <c r="C19" s="116"/>
+      <c r="D19" s="118"/>
+      <c r="E19" s="118"/>
+      <c r="F19" s="120"/>
+      <c r="G19" s="120"/>
+      <c r="H19" s="120"/>
+      <c r="I19" s="120"/>
+      <c r="J19" s="120"/>
+      <c r="K19" s="120"/>
+      <c r="L19" s="123"/>
+      <c r="M19" s="125"/>
+      <c r="N19" s="110"/>
+      <c r="O19" s="110"/>
+      <c r="P19" s="110"/>
+      <c r="Q19" s="110"/>
+      <c r="R19" s="110"/>
+      <c r="S19" s="100"/>
+      <c r="T19" s="102"/>
       <c r="U19" s="26"/>
       <c r="V19" s="26"/>
       <c r="W19" s="26"/>
@@ -6008,14 +6035,14 @@
       <c r="J20" s="22"/>
       <c r="K20" s="22"/>
       <c r="L20" s="22"/>
-      <c r="M20" s="84"/>
-      <c r="N20" s="77"/>
-      <c r="O20" s="77"/>
-      <c r="P20" s="77"/>
-      <c r="Q20" s="77"/>
-      <c r="R20" s="77"/>
-      <c r="S20" s="85"/>
-      <c r="T20" s="86"/>
+      <c r="M20" s="82"/>
+      <c r="N20" s="75"/>
+      <c r="O20" s="75"/>
+      <c r="P20" s="75"/>
+      <c r="Q20" s="75"/>
+      <c r="R20" s="75"/>
+      <c r="S20" s="83"/>
+      <c r="T20" s="84"/>
     </row>
     <row r="21" spans="1:244" ht="75.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="58"/>
@@ -6030,13 +6057,13 @@
       <c r="J21" s="49"/>
       <c r="K21" s="49"/>
       <c r="L21" s="65"/>
-      <c r="M21" s="87"/>
-      <c r="N21" s="88"/>
-      <c r="O21" s="88"/>
-      <c r="P21" s="88"/>
-      <c r="Q21" s="88"/>
-      <c r="R21" s="88"/>
-      <c r="S21" s="89"/>
+      <c r="M21" s="85"/>
+      <c r="N21" s="86"/>
+      <c r="O21" s="86"/>
+      <c r="P21" s="86"/>
+      <c r="Q21" s="86"/>
+      <c r="R21" s="86"/>
+      <c r="S21" s="87"/>
       <c r="T21" s="68"/>
       <c r="U21" s="26"/>
       <c r="V21" s="26"/>
@@ -6276,36 +6303,36 @@
       <c r="J22" s="22"/>
       <c r="K22" s="22"/>
       <c r="L22" s="22"/>
-      <c r="M22" s="84"/>
-      <c r="N22" s="77"/>
-      <c r="O22" s="77"/>
-      <c r="P22" s="77"/>
-      <c r="Q22" s="77"/>
-      <c r="R22" s="77"/>
-      <c r="S22" s="85"/>
-      <c r="T22" s="86"/>
+      <c r="M22" s="82"/>
+      <c r="N22" s="75"/>
+      <c r="O22" s="75"/>
+      <c r="P22" s="75"/>
+      <c r="Q22" s="75"/>
+      <c r="R22" s="75"/>
+      <c r="S22" s="83"/>
+      <c r="T22" s="84"/>
     </row>
     <row r="23" spans="1:244" ht="52.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="141"/>
-      <c r="B23" s="122"/>
-      <c r="C23" s="122"/>
-      <c r="D23" s="131"/>
-      <c r="E23" s="131"/>
-      <c r="F23" s="128"/>
-      <c r="G23" s="128"/>
-      <c r="H23" s="128"/>
-      <c r="I23" s="128"/>
-      <c r="J23" s="128"/>
-      <c r="K23" s="128"/>
-      <c r="L23" s="135"/>
-      <c r="M23" s="137"/>
-      <c r="N23" s="126"/>
-      <c r="O23" s="126"/>
-      <c r="P23" s="126"/>
-      <c r="Q23" s="126"/>
-      <c r="R23" s="126"/>
-      <c r="S23" s="126"/>
-      <c r="T23" s="147"/>
+      <c r="A23" s="115"/>
+      <c r="B23" s="116"/>
+      <c r="C23" s="116"/>
+      <c r="D23" s="117"/>
+      <c r="E23" s="117"/>
+      <c r="F23" s="113"/>
+      <c r="G23" s="113"/>
+      <c r="H23" s="113"/>
+      <c r="I23" s="113"/>
+      <c r="J23" s="113"/>
+      <c r="K23" s="113"/>
+      <c r="L23" s="105"/>
+      <c r="M23" s="107"/>
+      <c r="N23" s="103"/>
+      <c r="O23" s="103"/>
+      <c r="P23" s="103"/>
+      <c r="Q23" s="103"/>
+      <c r="R23" s="103"/>
+      <c r="S23" s="103"/>
+      <c r="T23" s="97"/>
       <c r="U23" s="26"/>
       <c r="V23" s="26"/>
       <c r="W23" s="26"/>
@@ -6532,26 +6559,26 @@
       <c r="IJ23" s="26"/>
     </row>
     <row r="24" spans="1:244" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="141"/>
-      <c r="B24" s="122"/>
-      <c r="C24" s="122"/>
-      <c r="D24" s="132"/>
-      <c r="E24" s="132"/>
-      <c r="F24" s="129"/>
-      <c r="G24" s="129"/>
-      <c r="H24" s="129"/>
-      <c r="I24" s="129"/>
-      <c r="J24" s="129"/>
-      <c r="K24" s="129"/>
-      <c r="L24" s="136"/>
-      <c r="M24" s="138"/>
-      <c r="N24" s="127"/>
-      <c r="O24" s="127"/>
-      <c r="P24" s="127"/>
-      <c r="Q24" s="127"/>
-      <c r="R24" s="127"/>
-      <c r="S24" s="127"/>
-      <c r="T24" s="148"/>
+      <c r="A24" s="115"/>
+      <c r="B24" s="116"/>
+      <c r="C24" s="116"/>
+      <c r="D24" s="118"/>
+      <c r="E24" s="118"/>
+      <c r="F24" s="114"/>
+      <c r="G24" s="114"/>
+      <c r="H24" s="114"/>
+      <c r="I24" s="114"/>
+      <c r="J24" s="114"/>
+      <c r="K24" s="114"/>
+      <c r="L24" s="106"/>
+      <c r="M24" s="108"/>
+      <c r="N24" s="104"/>
+      <c r="O24" s="104"/>
+      <c r="P24" s="104"/>
+      <c r="Q24" s="104"/>
+      <c r="R24" s="104"/>
+      <c r="S24" s="104"/>
+      <c r="T24" s="98"/>
       <c r="U24" s="26"/>
       <c r="V24" s="26"/>
       <c r="W24" s="26"/>
@@ -6790,14 +6817,14 @@
       <c r="J25" s="22"/>
       <c r="K25" s="22"/>
       <c r="L25" s="22"/>
-      <c r="M25" s="84"/>
-      <c r="N25" s="77"/>
-      <c r="O25" s="77"/>
-      <c r="P25" s="77"/>
-      <c r="Q25" s="77"/>
-      <c r="R25" s="77"/>
-      <c r="S25" s="85"/>
-      <c r="T25" s="86"/>
+      <c r="M25" s="82"/>
+      <c r="N25" s="75"/>
+      <c r="O25" s="75"/>
+      <c r="P25" s="75"/>
+      <c r="Q25" s="75"/>
+      <c r="R25" s="75"/>
+      <c r="S25" s="83"/>
+      <c r="T25" s="84"/>
     </row>
     <row r="26" spans="1:244" ht="76.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="50"/>
@@ -6812,13 +6839,13 @@
       <c r="J26" s="49"/>
       <c r="K26" s="49"/>
       <c r="L26" s="65"/>
-      <c r="M26" s="87"/>
-      <c r="N26" s="88"/>
-      <c r="O26" s="88"/>
-      <c r="P26" s="88"/>
-      <c r="Q26" s="88"/>
-      <c r="R26" s="88"/>
-      <c r="S26" s="89"/>
+      <c r="M26" s="85"/>
+      <c r="N26" s="86"/>
+      <c r="O26" s="86"/>
+      <c r="P26" s="86"/>
+      <c r="Q26" s="86"/>
+      <c r="R26" s="86"/>
+      <c r="S26" s="87"/>
       <c r="T26" s="68"/>
       <c r="U26" s="26"/>
       <c r="V26" s="26"/>
@@ -7058,17 +7085,95 @@
       <c r="J27" s="22"/>
       <c r="K27" s="22"/>
       <c r="L27" s="22"/>
-      <c r="M27" s="90"/>
-      <c r="N27" s="91"/>
-      <c r="O27" s="91"/>
-      <c r="P27" s="91"/>
-      <c r="Q27" s="91"/>
-      <c r="R27" s="91"/>
-      <c r="S27" s="92"/>
-      <c r="T27" s="93"/>
+      <c r="M27" s="88"/>
+      <c r="N27" s="89"/>
+      <c r="O27" s="89"/>
+      <c r="P27" s="89"/>
+      <c r="Q27" s="89"/>
+      <c r="R27" s="89"/>
+      <c r="S27" s="90"/>
+      <c r="T27" s="91"/>
     </row>
   </sheetData>
   <mergeCells count="102">
+    <mergeCell ref="M1:T1"/>
+    <mergeCell ref="M2:M5"/>
+    <mergeCell ref="T2:T5"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:E5"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="H2:H5"/>
+    <mergeCell ref="I2:I5"/>
+    <mergeCell ref="K2:K5"/>
+    <mergeCell ref="S2:S5"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="N2:N5"/>
+    <mergeCell ref="O2:O5"/>
+    <mergeCell ref="P2:P5"/>
+    <mergeCell ref="Q2:Q5"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:D5"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="J2:J5"/>
+    <mergeCell ref="L2:L5"/>
+    <mergeCell ref="P12:P13"/>
+    <mergeCell ref="Q12:Q13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="R2:R5"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="N15:N16"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="K23:K24"/>
+    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="P18:P19"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
     <mergeCell ref="T23:T24"/>
     <mergeCell ref="S18:S19"/>
     <mergeCell ref="T18:T19"/>
@@ -7093,84 +7198,6 @@
     <mergeCell ref="M12:M13"/>
     <mergeCell ref="N12:N13"/>
     <mergeCell ref="O12:O13"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="J23:J24"/>
-    <mergeCell ref="R18:R19"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="J18:J19"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="L18:L19"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="K23:K24"/>
-    <mergeCell ref="N18:N19"/>
-    <mergeCell ref="O18:O19"/>
-    <mergeCell ref="P18:P19"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="K15:K16"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="M15:M16"/>
-    <mergeCell ref="N15:N16"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="P12:P13"/>
-    <mergeCell ref="Q12:Q13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="R2:R5"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:D5"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="J2:J5"/>
-    <mergeCell ref="L2:L5"/>
-    <mergeCell ref="M1:T1"/>
-    <mergeCell ref="M2:M5"/>
-    <mergeCell ref="T2:T5"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:E5"/>
-    <mergeCell ref="F1:K1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="F2:F5"/>
-    <mergeCell ref="G2:G5"/>
-    <mergeCell ref="H2:H5"/>
-    <mergeCell ref="I2:I5"/>
-    <mergeCell ref="K2:K5"/>
-    <mergeCell ref="S2:S5"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="N2:N5"/>
-    <mergeCell ref="O2:O5"/>
-    <mergeCell ref="P2:P5"/>
-    <mergeCell ref="Q2:Q5"/>
   </mergeCells>
   <conditionalFormatting sqref="N10:S10 H10">
     <cfRule type="cellIs" priority="5" operator="equal">

</xml_diff>